<commit_message>
If condition -- launching browser -- screenshot file
</commit_message>
<xml_diff>
--- a/test_data/orange_data.xlsx
+++ b/test_data/orange_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="23895" windowHeight="9990"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="23895" windowHeight="9990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddEmercencyContact" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>${userename}</t>
   </si>
@@ -46,6 +46,24 @@
   </si>
   <si>
     <t>Lok</t>
+  </si>
+  <si>
+    <t>${username}</t>
+  </si>
+  <si>
+    <t>${membership}</t>
+  </si>
+  <si>
+    <t>${subscription_paid_by}</t>
+  </si>
+  <si>
+    <t>${subscription_amount}</t>
+  </si>
+  <si>
+    <t>${currency}</t>
+  </si>
+  <si>
+    <t>${commence_date}</t>
   </si>
 </sst>
 </file>
@@ -379,7 +397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -450,12 +468,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>